<commit_message>
spring is in the books
</commit_message>
<xml_diff>
--- a/Spring23_Grades.xlsx
+++ b/Spring23_Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rashap/Documents/MSE/ENGR2910/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17976483-18C3-0D48-BD04-0A55AC316AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9935A486-A773-4441-9A64-96CF2C7CE529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23420" yWindow="2080" windowWidth="20720" windowHeight="17440" xr2:uid="{47D13744-5F57-6A4B-8CFE-C4A7E62258B8}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16860" xr2:uid="{47D13744-5F57-6A4B-8CFE-C4A7E62258B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="20">
   <si>
     <t>Exam1</t>
   </si>
@@ -81,12 +81,30 @@
   </si>
   <si>
     <t>Assume 100%</t>
+  </si>
+  <si>
+    <t>Final Grade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letter Grade </t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -110,12 +128,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -145,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,13 +192,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +543,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,125 +555,152 @@
     <col min="2" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="5" width="15.33203125" customWidth="1"/>
     <col min="6" max="7" width="16" customWidth="1"/>
-    <col min="8" max="10" width="18.6640625" customWidth="1"/>
+    <col min="8" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="K1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="D2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6">
-        <v>97.86</v>
-      </c>
-      <c r="C3" s="6">
-        <v>100</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="B3" s="10">
+        <v>98.22</v>
+      </c>
+      <c r="C3" s="10">
+        <v>115</v>
+      </c>
+      <c r="D3" s="10">
         <v>74</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="10">
         <f>D3 + (100-D3)/4</f>
         <v>80.5</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10">
         <v>65</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6">
+      <c r="H3" s="10">
+        <v>64</v>
+      </c>
+      <c r="I3" s="10">
+        <f>H3 + (100-H3)/4</f>
+        <v>73</v>
+      </c>
+      <c r="J3" s="15">
         <f>((0.2*B3)+(0.1*C3)+(0.2*E3)+(0.2*G3))/(0.7)</f>
-        <v>83.817142857142869</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
+        <v>86.062857142857155</v>
+      </c>
+      <c r="K3" s="12">
+        <f>((0.2*B3)+(0.1*C3)+(0.2*E3)+(0.2*G3)+(0.3*I3))/(1)</f>
+        <v>82.144000000000005</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="16"/>
+    </row>
+    <row r="5" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="2" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="16"/>
+    </row>
+    <row r="6" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
         <v>14</v>
@@ -633,164 +723,200 @@
       <c r="I6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="J6" s="15"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="16"/>
+    </row>
+    <row r="7" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
-        <v>89.43</v>
-      </c>
-      <c r="C7" s="6">
-        <v>100</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="B7" s="5">
+        <v>89.11</v>
+      </c>
+      <c r="C7" s="5">
+        <v>115</v>
+      </c>
+      <c r="D7" s="5">
         <v>72</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <f>D7 + (100-D7)/4</f>
         <v>79</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
         <v>65</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6">
+      <c r="H7" s="5">
+        <v>55.5</v>
+      </c>
+      <c r="I7" s="5">
+        <f>H7 + (100-H7)/4</f>
+        <v>66.625</v>
+      </c>
+      <c r="J7" s="15">
         <f>((0.2*B7)+(0.1*C7)+(0.2*E7)+(0.2*G7))/(0.7)</f>
-        <v>80.980000000000018</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="2" t="s">
+        <v>83.031428571428577</v>
+      </c>
+      <c r="K7" s="13">
+        <f>((0.2*B7)+(0.1*C7)+(0.2*E7)+(0.2*G7)+(0.3*I7))/(1)</f>
+        <v>78.109499999999997</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="16"/>
+    </row>
+    <row r="9" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9"/>
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="2" t="s">
+      <c r="I9" s="11"/>
+      <c r="J9" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3" t="s">
+      <c r="K9" s="12"/>
+      <c r="L9" s="16"/>
+    </row>
+    <row r="10" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="D10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="6">
-        <v>93.21</v>
-      </c>
-      <c r="C11" s="6">
-        <v>100</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="B11" s="10">
+        <v>92.94</v>
+      </c>
+      <c r="C11" s="10">
+        <v>115</v>
+      </c>
+      <c r="D11" s="10">
         <v>65</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="10">
         <f>D11 + (100-D11)/4</f>
         <v>73.75</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
         <v>65</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6">
+      <c r="H11" s="10">
+        <v>68</v>
+      </c>
+      <c r="I11" s="10">
+        <f>H11 + (100-H11)/4</f>
+        <v>76</v>
+      </c>
+      <c r="J11" s="15">
         <f>((0.2*B11)+(0.1*C11)+(0.2*E11)+(0.2*G11))/(0.7)</f>
-        <v>80.56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
+        <v>82.625714285714295</v>
+      </c>
+      <c r="K11" s="12">
+        <f>((0.2*B11)+(0.1*C11)+(0.2*E11)+(0.2*G11)+(0.3*I11))/(1)</f>
+        <v>80.638000000000005</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="16"/>
+    </row>
+    <row r="13" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="2" t="s">
+      <c r="I13" s="6"/>
+      <c r="J13" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="16"/>
+    </row>
+    <row r="14" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3" t="s">
         <v>14</v>
@@ -813,168 +939,204 @@
       <c r="I14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="J14" s="15"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="16"/>
+    </row>
+    <row r="15" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="6">
-        <v>96.86</v>
-      </c>
-      <c r="C15" s="6">
+      <c r="B15" s="5">
+        <v>96.89</v>
+      </c>
+      <c r="C15" s="5">
         <v>100</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>99</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <f>D15 + (100-D15)/4</f>
         <v>99.25</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>83</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>87</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6">
+      <c r="H15" s="5">
+        <v>90</v>
+      </c>
+      <c r="I15" s="5">
+        <f>H15 + (100-H15)/4</f>
+        <v>92.5</v>
+      </c>
+      <c r="J15" s="15">
         <f>((0.2*B15)+(0.1*C15)+(0.2*E15)+(0.2*G15))/(0.7)</f>
-        <v>95.174285714285716</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="2" t="s">
+        <v>95.182857142857145</v>
+      </c>
+      <c r="K15" s="13">
+        <f>((0.2*B15)+(0.1*C15)+(0.2*E15)+(0.2*G15)+(0.3*I15))/(1)</f>
+        <v>94.378</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="17" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
+      <c r="E17" s="11"/>
+      <c r="F17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4" t="s">
+      <c r="G17" s="11"/>
+      <c r="H17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="2" t="s">
+      <c r="I17" s="11"/>
+      <c r="J17" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3" t="s">
+      <c r="K17" s="12"/>
+      <c r="L17" s="16"/>
+    </row>
+    <row r="18" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="D18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="16"/>
+    </row>
+    <row r="19" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="6">
-        <v>88.93</v>
-      </c>
-      <c r="C19" s="6">
+      <c r="B19" s="10">
+        <v>89.83</v>
+      </c>
+      <c r="C19" s="10">
         <v>100</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="10">
         <v>103</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="10">
         <f>D19</f>
         <v>103</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="10">
         <v>93</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="10">
         <v>95</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6">
+      <c r="H19" s="10">
+        <v>75</v>
+      </c>
+      <c r="I19" s="10">
+        <f>H19 + (100-H19)/4</f>
+        <v>81.25</v>
+      </c>
+      <c r="J19" s="15">
         <f>((0.2*B19)+(0.1*C19)+(0.2*E19)+(0.2*G19))/(0.7)</f>
-        <v>96.265714285714282</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
+        <v>96.522857142857148</v>
+      </c>
+      <c r="K19" s="12">
+        <f>((0.2*B19)+(0.1*C19)+(0.2*E19)+(0.2*G19)+(0.3*I19))/(1)</f>
+        <v>91.941000000000003</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="16"/>
+    </row>
+    <row r="21" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4" t="s">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="2" t="s">
+      <c r="I21" s="6"/>
+      <c r="J21" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="16"/>
+    </row>
+    <row r="22" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3" t="s">
         <v>14</v>
@@ -997,34 +1159,48 @@
       <c r="I22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="J22" s="15"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="16"/>
+    </row>
+    <row r="23" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="6">
-        <v>94.29</v>
-      </c>
-      <c r="C23" s="6">
+      <c r="B23" s="5">
+        <v>94.44</v>
+      </c>
+      <c r="C23" s="5">
         <v>100</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>80</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <f>D23 + (100-D23)/4</f>
         <v>85</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6">
+      <c r="F23" s="5"/>
+      <c r="G23" s="5">
         <v>65</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6">
+      <c r="H23" s="5">
+        <v>62</v>
+      </c>
+      <c r="I23" s="5">
+        <f>H23 + (100-H23)/4</f>
+        <v>71.5</v>
+      </c>
+      <c r="J23" s="15">
         <f>((0.2*B23)+(0.1*C23)+(0.2*E23)+(0.2*G23))/(0.7)</f>
-        <v>84.082857142857151</v>
+        <v>84.125714285714295</v>
+      </c>
+      <c r="K23" s="13">
+        <f>((0.2*B23)+(0.1*C23)+(0.2*E23)+(0.2*G23)+(0.3*I23))/(1)</f>
+        <v>80.338000000000008</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1032,24 +1208,24 @@
     <sortCondition ref="A3:A23"/>
   </sortState>
   <mergeCells count="18">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>